<commit_message>
Update HLR For Luma (Magento.softwaretestingboard.com).xlsx
</commit_message>
<xml_diff>
--- a/HLR For Luma/HLR For Luma (Magento.softwaretestingboard.com).xlsx
+++ b/HLR For Luma/HLR For Luma (Magento.softwaretestingboard.com).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36968C7A-A0BC-41AD-BEF9-A9362C8DF8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD50993B-100A-4119-91C1-EF52EF952F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Functionality ID</t>
   </si>
@@ -157,9 +157,6 @@
     <t>while clickiing on product size boxes, its working properly</t>
   </si>
   <si>
-    <t>while clickinig on product color option, its working properly</t>
-  </si>
-  <si>
     <t>while put number of qty in box its working properly</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>to check Add to wish list button</t>
   </si>
   <si>
-    <t>while click on add to wish list button, working proper</t>
-  </si>
-  <si>
     <t>to check add to compare button</t>
   </si>
   <si>
@@ -266,6 +260,33 @@
   </si>
   <si>
     <t>while cliking on compare product text link, showing proper result</t>
+  </si>
+  <si>
+    <t>while click on add to wish list button, working properly</t>
+  </si>
+  <si>
+    <t>while clickinig on product color option, its not working properly</t>
+  </si>
+  <si>
+    <t>to check forgot your password text link</t>
+  </si>
+  <si>
+    <t>while clicking on to check forgot your password, its working properly</t>
+  </si>
+  <si>
+    <t>to check reload captcha button</t>
+  </si>
+  <si>
+    <t>while clicking on reload captcha button, its working properly</t>
+  </si>
+  <si>
+    <t>to check reset my password button</t>
+  </si>
+  <si>
+    <t>while clicking on reset my password button, its working properly</t>
+  </si>
+  <si>
+    <t>bag</t>
   </si>
 </sst>
 </file>
@@ -372,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -407,6 +428,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -414,7 +438,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,11 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="6" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,28 +796,28 @@
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -814,7 +838,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -830,7 +854,7 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -839,419 +863,441 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>35</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>36</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>7</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>11</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>60</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>17</v>
-      </c>
-      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>75</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>77</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>90</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>100</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>120</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>21</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>22</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>28</v>
+        <v>140</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>34</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>62</v>
+      <c r="A43" s="15">
+        <v>160</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
-        <v>36</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>66</v>
+      <c r="A45" s="4">
+        <v>170</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>174</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>180</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>185</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="4">
+        <v>250</v>
+      </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
@@ -1314,6 +1360,26 @@
       <c r="A63" s="4"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>